<commit_message>
ECP-1184: adds some refinements and tests
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/sales_area_licences_OXF.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/sales_area_licences_OXF.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3FCFE58-39F0-6949-9C7A-733C91C77593}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615C3F40-331C-FF4D-8E12-A418739CF558}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Lease Reference</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Unit Reference</t>
   </si>
   <si>
-    <t>Start Date</t>
-  </si>
-  <si>
     <t>Sales Area Non Food</t>
   </si>
   <si>
@@ -62,6 +59,12 @@
   </si>
   <si>
     <t>OXF-001</t>
+  </si>
+  <si>
+    <t>Occupancy Start Date</t>
+  </si>
+  <si>
+    <t>License Start Date</t>
   </si>
 </sst>
 </file>
@@ -422,24 +425,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,87 +450,103 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="1">
         <v>39448</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
+        <v>39448</v>
+      </c>
+      <c r="E2" s="2">
         <v>100</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>10</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>41585</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2">
+      <c r="D3" s="1">
+        <v>41640</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
         <v>22</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>40544</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="1">
+        <v>40544</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>40374</v>
       </c>
-      <c r="D5" s="2">
-        <v>200.25</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="D5" s="1">
+        <v>43876</v>
+      </c>
+      <c r="E5" s="2">
+        <v>201.33</v>
+      </c>
       <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>